<commit_message>
Needs to activate security, needs to add records to firebase, & connect to frontend with security
</commit_message>
<xml_diff>
--- a/functions/pdf_generator/data/data_payslip.xlsx
+++ b/functions/pdf_generator/data/data_payslip.xlsx
@@ -563,128 +563,126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>employee_name sample value</t>
+          <t>AMOGAS Data 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>address sample value</t>
+          <t>BELLO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>reference sample value</t>
+          <t>Sample Data 1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>employer_name sample value</t>
+          <t>Sample Data 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>email sample value</t>
+          <t>Sample Data 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>job_status sample value</t>
+          <t>sam17.bello@ymail.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>deminimis sample value</t>
+          <t>Sample data 2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>basic_salary sample value</t>
+          <t>Sample data 2</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>overtime sample value</t>
+          <t>Sample data 2</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>gross_pay sample value</t>
+          <t>Sample data 2</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>net_pay sample value</t>
+          <t>PHP 300</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>tax sample value</t>
+          <t>PHP 20000</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>sss sample value</t>
+          <t>FINAL PHP 20000</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>loan sample value</t>
+          <t>₱26502.00</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>philhealth_payment sample value</t>
+          <t>₱857.61</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>hdmf sample value</t>
+          <t>₱1192.59</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>deductions sample value</t>
+          <t>PHP 200321300</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>postcode sample value</t>
+          <t>₱88.34</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>gender sample value</t>
+          <t>₱100.00</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>grade sample value</t>
+          <t>₱2258.54</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>department sample value</t>
+          <t>₱24243.46</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>pay_date sample value</t>
+          <t>Sample data 2</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>philhealth_number sample value</t>
+          <t>₱857.61</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>taxable_pay sample value</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>pension_pay sample value</t>
-        </is>
+          <t>₱1192.59</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>